<commit_message>
-Fixed the fifth algorithm -Changed the picture of the performance graph
</commit_message>
<xml_diff>
--- a/Algorithms/Fifth/График.xlsx
+++ b/Algorithms/Fifth/График.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CLionProjects\Algorithms\Algorithms\Fifth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EC1798C6-BBCA-4D05-AA5E-C6CEB22E17A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45EBBBE7-5AF9-4B86-B444-9FB93CADDAC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{C7C89AFE-CE28-457C-9CCB-18A6C5ABDA77}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>lenght</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>map</t>
+  </si>
+  <si>
+    <t>0.000000</t>
   </si>
 </sst>
 </file>
@@ -74,7 +77,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -97,16 +100,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -249,10 +269,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$21</c:f>
+              <c:f>Лист1!$A$2:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -312,75 +332,81 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>950000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$B$2:$B$21</c:f>
+              <c:f>Лист1!$B$2:$B$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52.857700000000001</c:v>
+                  <c:v>27.927900000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>102.7525</c:v>
+                  <c:v>58.842599999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>145.58449999999999</c:v>
+                  <c:v>85.742400000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>194.48179999999999</c:v>
+                  <c:v>116.6883</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>264.26560000000001</c:v>
+                  <c:v>146.65899999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>301.14089999999999</c:v>
+                  <c:v>195.44900000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>334.8587</c:v>
+                  <c:v>204.49510000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>383.16340000000002</c:v>
+                  <c:v>249.01079999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>432.38220000000001</c:v>
+                  <c:v>267.2851</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>485.4692</c:v>
+                  <c:v>293.90309999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>537.72929999999997</c:v>
+                  <c:v>327.66590000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>587.91539999999998</c:v>
+                  <c:v>349.91879999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>621.84379999999999</c:v>
+                  <c:v>381.3211</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>669.92250000000001</c:v>
+                  <c:v>414.05459999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>718.01700000000005</c:v>
+                  <c:v>439.52600000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>769.23260000000005</c:v>
+                  <c:v>464.05520000000001</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>822.34619999999995</c:v>
+                  <c:v>512.83140000000003</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>889.23230000000001</c:v>
+                  <c:v>525.59249999999997</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>914.85850000000005</c:v>
+                  <c:v>576.08190000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>619.71619999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -420,10 +446,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Лист1!$A$2:$A$21</c:f>
+              <c:f>Лист1!$A$2:$A$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -483,75 +509,81 @@
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>950000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1000000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Лист1!$C$2:$C$21</c:f>
+              <c:f>Лист1!$C$2:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="20"/>
+                <c:ptCount val="21"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>38.897300000000001</c:v>
+                  <c:v>20.946100000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>78.790999999999997</c:v>
+                  <c:v>38.895400000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>109.2779</c:v>
+                  <c:v>55.851100000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>146.28139999999999</c:v>
+                  <c:v>73.802800000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>182.51140000000001</c:v>
+                  <c:v>90.820099999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>220.10570000000001</c:v>
+                  <c:v>110.7332</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>246.82689999999999</c:v>
+                  <c:v>124.49</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>280.42520000000002</c:v>
+                  <c:v>142.65710000000001</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>317.15210000000002</c:v>
+                  <c:v>158.57769999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>348.0677</c:v>
+                  <c:v>174.8108</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>393.04059999999998</c:v>
+                  <c:v>192.17930000000001</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>426.4024</c:v>
+                  <c:v>208.21420000000001</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>454.255</c:v>
+                  <c:v>227.08709999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>486.51429999999999</c:v>
+                  <c:v>240.7474</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>523.14930000000004</c:v>
+                  <c:v>262.99990000000003</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>555.23429999999996</c:v>
+                  <c:v>274.31810000000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>600.71249999999998</c:v>
+                  <c:v>291.72680000000003</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>625.80499999999995</c:v>
+                  <c:v>307.93920000000003</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>657.64089999999999</c:v>
+                  <c:v>325.60430000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>344.26420000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -578,6 +610,8 @@
         <c:axId val="1726016111"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1050000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1675,10 +1709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9313575A-FB03-4566-AFE5-6E330D4DA982}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1702,11 +1736,11 @@
       <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2">
-        <v>0</v>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1714,10 +1748,10 @@
         <v>50000</v>
       </c>
       <c r="B3" s="1">
-        <v>52.857700000000001</v>
+        <v>27.927900000000001</v>
       </c>
       <c r="C3" s="1">
-        <v>38.897300000000001</v>
+        <v>20.946100000000001</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1725,10 +1759,10 @@
         <v>100000</v>
       </c>
       <c r="B4" s="1">
-        <v>102.7525</v>
+        <v>58.842599999999997</v>
       </c>
       <c r="C4" s="1">
-        <v>78.790999999999997</v>
+        <v>38.895400000000002</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1736,10 +1770,10 @@
         <v>150000</v>
       </c>
       <c r="B5" s="1">
-        <v>145.58449999999999</v>
+        <v>85.742400000000004</v>
       </c>
       <c r="C5" s="1">
-        <v>109.2779</v>
+        <v>55.851100000000002</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1747,10 +1781,10 @@
         <v>200000</v>
       </c>
       <c r="B6" s="1">
-        <v>194.48179999999999</v>
+        <v>116.6883</v>
       </c>
       <c r="C6" s="1">
-        <v>146.28139999999999</v>
+        <v>73.802800000000005</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1758,10 +1792,10 @@
         <v>250000</v>
       </c>
       <c r="B7" s="1">
-        <v>264.26560000000001</v>
+        <v>146.65899999999999</v>
       </c>
       <c r="C7" s="1">
-        <v>182.51140000000001</v>
+        <v>90.820099999999996</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1769,10 +1803,10 @@
         <v>300000</v>
       </c>
       <c r="B8" s="1">
-        <v>301.14089999999999</v>
+        <v>195.44900000000001</v>
       </c>
       <c r="C8" s="1">
-        <v>220.10570000000001</v>
+        <v>110.7332</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1780,10 +1814,10 @@
         <v>350000</v>
       </c>
       <c r="B9" s="1">
-        <v>334.8587</v>
+        <v>204.49510000000001</v>
       </c>
       <c r="C9" s="1">
-        <v>246.82689999999999</v>
+        <v>124.49</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1791,10 +1825,10 @@
         <v>400000</v>
       </c>
       <c r="B10" s="1">
-        <v>383.16340000000002</v>
+        <v>249.01079999999999</v>
       </c>
       <c r="C10" s="1">
-        <v>280.42520000000002</v>
+        <v>142.65710000000001</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1802,10 +1836,10 @@
         <v>450000</v>
       </c>
       <c r="B11" s="1">
-        <v>432.38220000000001</v>
+        <v>267.2851</v>
       </c>
       <c r="C11" s="1">
-        <v>317.15210000000002</v>
+        <v>158.57769999999999</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1813,10 +1847,10 @@
         <v>500000</v>
       </c>
       <c r="B12" s="1">
-        <v>485.4692</v>
+        <v>293.90309999999999</v>
       </c>
       <c r="C12" s="1">
-        <v>348.0677</v>
+        <v>174.8108</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1824,10 +1858,10 @@
         <v>550000</v>
       </c>
       <c r="B13" s="1">
-        <v>537.72929999999997</v>
+        <v>327.66590000000002</v>
       </c>
       <c r="C13" s="1">
-        <v>393.04059999999998</v>
+        <v>192.17930000000001</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1835,10 +1869,10 @@
         <v>600000</v>
       </c>
       <c r="B14" s="1">
-        <v>587.91539999999998</v>
+        <v>349.91879999999998</v>
       </c>
       <c r="C14" s="1">
-        <v>426.4024</v>
+        <v>208.21420000000001</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1846,10 +1880,10 @@
         <v>650000</v>
       </c>
       <c r="B15" s="1">
-        <v>621.84379999999999</v>
+        <v>381.3211</v>
       </c>
       <c r="C15" s="1">
-        <v>454.255</v>
+        <v>227.08709999999999</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1857,10 +1891,10 @@
         <v>700000</v>
       </c>
       <c r="B16" s="1">
-        <v>669.92250000000001</v>
+        <v>414.05459999999999</v>
       </c>
       <c r="C16" s="1">
-        <v>486.51429999999999</v>
+        <v>240.7474</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1868,10 +1902,10 @@
         <v>750000</v>
       </c>
       <c r="B17" s="1">
-        <v>718.01700000000005</v>
+        <v>439.52600000000001</v>
       </c>
       <c r="C17" s="1">
-        <v>523.14930000000004</v>
+        <v>262.99990000000003</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1879,10 +1913,10 @@
         <v>800000</v>
       </c>
       <c r="B18" s="1">
-        <v>769.23260000000005</v>
+        <v>464.05520000000001</v>
       </c>
       <c r="C18" s="1">
-        <v>555.23429999999996</v>
+        <v>274.31810000000002</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1890,10 +1924,10 @@
         <v>850000</v>
       </c>
       <c r="B19" s="1">
-        <v>822.34619999999995</v>
+        <v>512.83140000000003</v>
       </c>
       <c r="C19" s="1">
-        <v>600.71249999999998</v>
+        <v>291.72680000000003</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1901,10 +1935,10 @@
         <v>900000</v>
       </c>
       <c r="B20" s="1">
-        <v>889.23230000000001</v>
+        <v>525.59249999999997</v>
       </c>
       <c r="C20" s="1">
-        <v>625.80499999999995</v>
+        <v>307.93920000000003</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1912,10 +1946,21 @@
         <v>950000</v>
       </c>
       <c r="B21" s="1">
-        <v>914.85850000000005</v>
+        <v>576.08190000000002</v>
       </c>
       <c r="C21" s="1">
-        <v>657.64089999999999</v>
+        <v>325.60430000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="B22" s="4">
+        <v>619.71619999999996</v>
+      </c>
+      <c r="C22" s="3">
+        <v>344.26420000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>